<commit_message>
changes done to xlsx file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganesh/Desktop/crop-yield-prediction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ganesh/Developer/gnevercodesz/crop-yield-prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A29227AF-FFA2-3D48-92D8-14DD4C141772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BAE107-8C10-C04C-A538-C41B92612CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11500" yWindow="1060" windowWidth="15740" windowHeight="17440" xr2:uid="{0C3FEEEC-24F7-A24B-898E-132164A0E8C9}"/>
   </bookViews>
@@ -53,9 +53,6 @@
     <t>240.0.0.0.</t>
   </si>
   <si>
-    <t>240.63.255.255.</t>
-  </si>
-  <si>
     <t>224.64.0.0.</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 224.64.16.36 </t>
+  </si>
+  <si>
+    <t>sdaasf</t>
   </si>
 </sst>
 </file>
@@ -153,9 +153,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +193,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -299,7 +299,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -441,7 +441,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -451,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E41BAB9-EA35-5A46-8D75-826F79E14496}">
   <dimension ref="A5:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="138" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +482,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>3</v>
@@ -490,10 +490,10 @@
     </row>
     <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -501,10 +501,10 @@
     </row>
     <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="12" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="13" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="14" spans="1:4" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
         <v>3</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2</v>

</xml_diff>